<commit_message>
Mise a jour Expression besoins et Lsite emplacements
</commit_message>
<xml_diff>
--- a/ListeEmplacements2020.xlsx
+++ b/ListeEmplacements2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\-- PROJET TP TD EN COURS DE REDACTIONS\____CDCHARGE PROJET VG\PROJET 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\-- PROJET TP TD EN COURS DE REDACTIONS\____CDCHARGE PROJET VG\PROJET 1\A FAIRE - Projet Vide Grenier V0.2 vers V0.3 WEB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294963C0-A76D-4F61-ACAC-008F30CE0F2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE70DC5-BA79-4F78-BB83-352D1D2D06BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9450" yWindow="1155" windowWidth="27780" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-2205" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>Emplacement de 4m</t>
   </si>
   <si>
-    <t>&lt; ou &gt; emplacement mors de 1m a gauche ou a droite</t>
-  </si>
-  <si>
     <t>ZD A</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   </si>
   <si>
     <t xml:space="preserve">soit </t>
+  </si>
+  <si>
+    <t>&lt; ou &gt; emplacement mords de 1m a gauche ou a droite</t>
   </si>
 </sst>
 </file>
@@ -874,16 +874,16 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1203,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD372"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AT30" sqref="AT30"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AY15" sqref="AY15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,7 +1248,7 @@
       <c r="AT2"/>
       <c r="AV2" s="44"/>
       <c r="AW2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1274,7 +1274,7 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="V4" s="35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="W4" s="35"/>
       <c r="X4" s="6"/>
@@ -1304,7 +1304,7 @@
       <c r="B5" s="3"/>
       <c r="I5" s="40"/>
       <c r="J5" s="37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>9</v>
@@ -1319,37 +1319,37 @@
         <v>10</v>
       </c>
       <c r="O5" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="U5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="V5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="W5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="X5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y5" s="36" t="s">
         <v>43</v>
-      </c>
-      <c r="P5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="S5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="T5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="U5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="V5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="W5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="X5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y5" s="36" t="s">
-        <v>44</v>
       </c>
       <c r="Z5" s="10" t="s">
         <v>9</v>
@@ -1367,10 +1367,10 @@
         <v>11</v>
       </c>
       <c r="AE5" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF5" s="36" t="s">
         <v>45</v>
-      </c>
-      <c r="AF5" s="36" t="s">
-        <v>46</v>
       </c>
       <c r="AG5" s="12" t="s">
         <v>12</v>
@@ -1382,7 +1382,7 @@
         <v>9</v>
       </c>
       <c r="AJ5" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AK5" s="15" t="s">
         <v>13</v>
@@ -1391,7 +1391,7 @@
         <v>11</v>
       </c>
       <c r="AM5" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AN5" s="16" t="s">
         <v>9</v>
@@ -1433,7 +1433,7 @@
       <c r="V6" s="45"/>
       <c r="W6" s="46"/>
       <c r="X6" s="44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Y6" s="44"/>
       <c r="Z6" s="44"/>
@@ -1580,36 +1580,36 @@
       </c>
       <c r="K8" s="44"/>
       <c r="M8" s="43"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="48"/>
-      <c r="U8" s="48"/>
-      <c r="V8" s="48"/>
-      <c r="W8" s="48"/>
-      <c r="X8" s="48"/>
-      <c r="Y8" s="48"/>
-      <c r="Z8" s="48"/>
-      <c r="AA8" s="48"/>
-      <c r="AB8" s="48"/>
-      <c r="AC8" s="48"/>
-      <c r="AD8" s="48"/>
-      <c r="AE8" s="48"/>
-      <c r="AF8" s="48"/>
-      <c r="AG8" s="48"/>
-      <c r="AH8" s="48"/>
-      <c r="AI8" s="48"/>
-      <c r="AJ8" s="48"/>
-      <c r="AK8" s="48"/>
-      <c r="AL8" s="48"/>
-      <c r="AM8" s="48"/>
-      <c r="AN8" s="48"/>
-      <c r="AO8" s="48"/>
-      <c r="AP8" s="48"/>
-      <c r="AQ8" s="48"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="50"/>
+      <c r="S8" s="50"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="50"/>
+      <c r="V8" s="50"/>
+      <c r="W8" s="50"/>
+      <c r="X8" s="50"/>
+      <c r="Y8" s="50"/>
+      <c r="Z8" s="50"/>
+      <c r="AA8" s="50"/>
+      <c r="AB8" s="50"/>
+      <c r="AC8" s="50"/>
+      <c r="AD8" s="50"/>
+      <c r="AE8" s="50"/>
+      <c r="AF8" s="50"/>
+      <c r="AG8" s="50"/>
+      <c r="AH8" s="50"/>
+      <c r="AI8" s="50"/>
+      <c r="AJ8" s="50"/>
+      <c r="AK8" s="50"/>
+      <c r="AL8" s="50"/>
+      <c r="AM8" s="50"/>
+      <c r="AN8" s="50"/>
+      <c r="AO8" s="50"/>
+      <c r="AP8" s="50"/>
+      <c r="AQ8" s="50"/>
       <c r="AR8" s="3"/>
       <c r="AS8"/>
       <c r="AT8"/>
@@ -1626,25 +1626,25 @@
       <c r="A9" s="9"/>
       <c r="B9" s="3"/>
       <c r="C9" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="E9" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="G9" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="36" t="s">
+      <c r="I9" s="36" t="s">
         <v>65</v>
-      </c>
-      <c r="H9" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="36" t="s">
-        <v>66</v>
       </c>
       <c r="J9" s="39" t="s">
         <v>9</v>
@@ -1964,10 +1964,10 @@
       </c>
       <c r="AU12"/>
       <c r="AV12" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="AX12" s="19" t="s">
         <v>39</v>
-      </c>
-      <c r="AX12" s="19" t="s">
-        <v>40</v>
       </c>
       <c r="AY12" s="2"/>
     </row>
@@ -2203,29 +2203,29 @@
         <v>10</v>
       </c>
       <c r="H16" s="28"/>
-      <c r="I16" s="50" t="s">
+      <c r="I16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="50" t="s">
+      <c r="J16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="50" t="s">
+      <c r="K16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="50" t="s">
+      <c r="L16" s="48" t="s">
         <v>20</v>
       </c>
       <c r="M16" s="28"/>
-      <c r="N16" s="50" t="s">
+      <c r="N16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="O16" s="50" t="s">
+      <c r="O16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="P16" s="50" t="s">
+      <c r="P16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="Q16" s="50" t="s">
+      <c r="Q16" s="48" t="s">
         <v>20</v>
       </c>
       <c r="R16" s="28"/>
@@ -2249,49 +2249,49 @@
         <v>29</v>
       </c>
       <c r="AB16" s="28"/>
-      <c r="AC16" s="50" t="s">
+      <c r="AC16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="AD16" s="50" t="s">
+      <c r="AD16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="AE16" s="50" t="s">
+      <c r="AE16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="AF16" s="50" t="s">
+      <c r="AF16" s="48" t="s">
         <v>20</v>
       </c>
       <c r="AG16" s="28"/>
-      <c r="AH16" s="50" t="s">
+      <c r="AH16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="AI16" s="50" t="s">
+      <c r="AI16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="AJ16" s="50" t="s">
+      <c r="AJ16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="AK16" s="50" t="s">
+      <c r="AK16" s="48" t="s">
         <v>20</v>
       </c>
       <c r="AL16" s="28"/>
-      <c r="AM16" s="50" t="s">
+      <c r="AM16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="AN16" s="50" t="s">
+      <c r="AN16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="AO16" s="50" t="s">
+      <c r="AO16" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="AP16" s="50" t="s">
-        <v>61</v>
+      <c r="AP16" s="48" t="s">
+        <v>60</v>
       </c>
       <c r="AQ16" s="28"/>
       <c r="AR16" s="3"/>
       <c r="AT16"/>
       <c r="AV16" s="31" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:56" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2311,15 +2311,15 @@
         <v>2</v>
       </c>
       <c r="H17" s="30"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
       <c r="M17" s="30"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="51"/>
-      <c r="P17" s="51"/>
-      <c r="Q17" s="51"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
       <c r="R17" s="30"/>
       <c r="S17" s="4" t="s">
         <v>2</v>
@@ -2349,20 +2349,20 @@
         <v>29</v>
       </c>
       <c r="AB17" s="30"/>
-      <c r="AC17" s="51"/>
-      <c r="AD17" s="51"/>
-      <c r="AE17" s="51"/>
-      <c r="AF17" s="51"/>
+      <c r="AC17" s="49"/>
+      <c r="AD17" s="49"/>
+      <c r="AE17" s="49"/>
+      <c r="AF17" s="49"/>
       <c r="AG17" s="30"/>
-      <c r="AH17" s="51"/>
-      <c r="AI17" s="51"/>
-      <c r="AJ17" s="51"/>
-      <c r="AK17" s="51"/>
+      <c r="AH17" s="49"/>
+      <c r="AI17" s="49"/>
+      <c r="AJ17" s="49"/>
+      <c r="AK17" s="49"/>
       <c r="AL17" s="30"/>
-      <c r="AM17" s="51"/>
-      <c r="AN17" s="51"/>
-      <c r="AO17" s="51"/>
-      <c r="AP17" s="51"/>
+      <c r="AM17" s="49"/>
+      <c r="AN17" s="49"/>
+      <c r="AO17" s="49"/>
+      <c r="AP17" s="49"/>
       <c r="AQ17" s="30"/>
       <c r="AR17" s="3"/>
       <c r="AT17" s="2"/>
@@ -2374,48 +2374,48 @@
     <row r="18" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="3"/>
-      <c r="I18" s="49" t="s">
+      <c r="I18" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="N18" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="J18" s="49"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="49"/>
-      <c r="N18" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="O18" s="49"/>
-      <c r="P18" s="49"/>
-      <c r="Q18" s="49"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="51"/>
       <c r="AA18" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="AC18" s="49" t="s">
+      <c r="AC18" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD18" s="51"/>
+      <c r="AE18" s="51"/>
+      <c r="AF18" s="51"/>
+      <c r="AH18" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="AD18" s="49"/>
-      <c r="AE18" s="49"/>
-      <c r="AF18" s="49"/>
-      <c r="AH18" s="49" t="s">
+      <c r="AI18" s="51"/>
+      <c r="AJ18" s="51"/>
+      <c r="AK18" s="51"/>
+      <c r="AM18" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="AI18" s="49"/>
-      <c r="AJ18" s="49"/>
-      <c r="AK18" s="49"/>
-      <c r="AM18" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN18" s="49"/>
-      <c r="AO18" s="49"/>
-      <c r="AP18" s="49"/>
+      <c r="AN18" s="51"/>
+      <c r="AO18" s="51"/>
+      <c r="AP18" s="51"/>
       <c r="AR18" s="3"/>
       <c r="AT18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU18">
         <v>163</v>
       </c>
       <c r="AV18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2484,16 +2484,16 @@
       </c>
       <c r="AI20" s="33"/>
       <c r="AJ20" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AL20" s="33"/>
       <c r="AM20" s="33"/>
       <c r="AN20" s="33"/>
       <c r="AP20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR20" t="s">
         <v>53</v>
-      </c>
-      <c r="AR20" t="s">
-        <v>54</v>
       </c>
       <c r="AT20"/>
     </row>
@@ -2502,7 +2502,7 @@
         <v>29</v>
       </c>
       <c r="AN21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AP21">
         <v>2</v>
@@ -2563,7 +2563,7 @@
         <v>26</v>
       </c>
       <c r="AT27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AW27" s="2"/>
       <c r="AY27"/>
@@ -2576,7 +2576,7 @@
         <v>44</v>
       </c>
       <c r="AT28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AY28"/>
     </row>
@@ -2588,14 +2588,14 @@
         <v>13</v>
       </c>
       <c r="AT29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AW29" s="2"/>
       <c r="AY29"/>
     </row>
     <row r="30" spans="1:56" x14ac:dyDescent="0.25">
       <c r="AT30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AW30" s="2"/>
       <c r="AY30"/>
@@ -3628,16 +3628,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AE16:AE17"/>
-    <mergeCell ref="AM16:AM17"/>
-    <mergeCell ref="AN16:AN17"/>
-    <mergeCell ref="AO16:AO17"/>
-    <mergeCell ref="AP16:AP17"/>
-    <mergeCell ref="AF16:AF17"/>
-    <mergeCell ref="AH16:AH17"/>
-    <mergeCell ref="AI16:AI17"/>
-    <mergeCell ref="AJ16:AJ17"/>
-    <mergeCell ref="AK16:AK17"/>
     <mergeCell ref="N8:AQ8"/>
     <mergeCell ref="I18:L18"/>
     <mergeCell ref="N18:Q18"/>
@@ -3654,6 +3644,16 @@
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="AC16:AC17"/>
     <mergeCell ref="AD16:AD17"/>
+    <mergeCell ref="AE16:AE17"/>
+    <mergeCell ref="AM16:AM17"/>
+    <mergeCell ref="AN16:AN17"/>
+    <mergeCell ref="AO16:AO17"/>
+    <mergeCell ref="AP16:AP17"/>
+    <mergeCell ref="AF16:AF17"/>
+    <mergeCell ref="AH16:AH17"/>
+    <mergeCell ref="AI16:AI17"/>
+    <mergeCell ref="AJ16:AJ17"/>
+    <mergeCell ref="AK16:AK17"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>

</xml_diff>